<commit_message>
add quaternary design, rename function & variable names according to google C++ standard
</commit_message>
<xml_diff>
--- a/DesignDocs/C1 符号表设计.xlsx
+++ b/DesignDocs/C1 符号表设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t>符号表设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -219,6 +219,18 @@
   </si>
   <si>
     <t>对不符合语义结构的单词，进行错误局部化处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quaternaryAddress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应四元式的标号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -583,15 +595,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.25" customWidth="1"/>
@@ -882,72 +894,101 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
+        <v>3</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24">
         <v>5</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>